<commit_message>
update spreadsheet, add screenshot
</commit_message>
<xml_diff>
--- a/complexity.xlsx
+++ b/complexity.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="22035" windowHeight="9540"/>
+    <workbookView xWindow="345" yWindow="255" windowWidth="17385" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -86,14 +86,205 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -399,256 +590,291 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="11" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="11" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8"/>
+      <c r="B1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="10"/>
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="I1" s="10"/>
+      <c r="J1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="10"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="12">
         <f>COMBIN(2,1)*COMBIN(1,1)/2</f>
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="13">
         <f>B3*2</f>
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="12">
         <f>COMBIN(4,1)*COMBIN(3,1)/2</f>
         <v>6</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="13">
         <f>D3*4</f>
         <v>24</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="12">
         <f>COMBIN(8,1)*COMBIN(7,1)/2</f>
         <v>28</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="13">
         <f>F3*8</f>
         <v>224</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="12">
         <f>COMBIN(16,1)*COMBIN(15,1)/2</f>
         <v>120</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="13">
         <f>H3*16</f>
         <v>1920</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="12">
         <f>COMBIN(32,1)*COMBIN(31,1)/2</f>
         <v>496</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="13">
         <f>J3*32</f>
         <v>15872</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="2">
         <f>COMBIN(4,2)*COMBIN(2,2)/2</f>
         <v>3</v>
       </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E7" si="0">D4*4</f>
+      <c r="E4" s="3">
+        <f t="shared" ref="E4" si="0">D4*4</f>
         <v>12</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <f>COMBIN(8,2)*COMBIN(6,2)/2</f>
         <v>210</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <f t="shared" ref="G4:G5" si="1">F4*8</f>
         <v>1680</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <f>COMBIN(16,2) * COMBIN(14,2)/2</f>
         <v>5460</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <f t="shared" ref="I4:I6" si="2">H4*16</f>
         <v>87360</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="2">
         <f xml:space="preserve"> COMBIN(32,2) * COMBIN(30,2)/2</f>
         <v>107880</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="3">
         <f t="shared" ref="K4:K7" si="3">J4*32</f>
         <v>3452160</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F5">
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="2">
         <f>COMBIN(8,4)*COMBIN(4,4)/2</f>
         <v>35</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <f t="shared" si="1"/>
         <v>280</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <f>COMBIN(16,4) * COMBIN(12,4)/2</f>
         <v>450450.00000000006</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="3">
         <f t="shared" si="2"/>
         <v>7207200.0000000009</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="2">
         <f>COMBIN(32,4) * COMBIN(28,4)/2</f>
         <v>368140500</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="3">
         <f t="shared" si="3"/>
         <v>11780496000</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H6">
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="2">
         <f>COMBIN(16,8)*COMBIN(8,8)/2</f>
         <v>6434.9999999999991</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="3">
         <f t="shared" si="2"/>
         <v>102959.99999999999</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="2">
         <f>COMBIN(32,8) * COMBIN(24,8)/2</f>
         <v>3867952309649.9995</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="3">
         <f t="shared" si="3"/>
         <v>123774473908799.98</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J7">
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="2">
         <f>COMBIN(32,16) * COMBIN(16,16)/2</f>
         <v>300540195</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="3">
         <f t="shared" si="3"/>
         <v>9617286240</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
-        <f>SUM(B3:B7)</f>
+      <c r="B9" s="4">
+        <f t="shared" ref="B9:K9" si="4">SUM(B3:B7)</f>
         <v>1</v>
       </c>
-      <c r="C9">
-        <f>SUM(C3:C7)</f>
+      <c r="C9" s="5">
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="D9">
-        <f>SUM(D3:D7)</f>
+      <c r="D9" s="4">
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="E9">
-        <f>SUM(E3:E7)</f>
+      <c r="E9" s="5">
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
-      <c r="F9">
-        <f>SUM(F3:F7)</f>
+      <c r="F9" s="4">
+        <f t="shared" si="4"/>
         <v>273</v>
       </c>
-      <c r="G9">
-        <f>SUM(G3:G7)</f>
+      <c r="G9" s="5">
+        <f t="shared" si="4"/>
         <v>2184</v>
       </c>
-      <c r="H9">
-        <f>SUM(H3:H7)</f>
+      <c r="H9" s="4">
+        <f t="shared" si="4"/>
         <v>462465.00000000006</v>
       </c>
-      <c r="I9">
-        <f>SUM(I3:I7)</f>
+      <c r="I9" s="5">
+        <f t="shared" si="4"/>
         <v>7399440.0000000009</v>
       </c>
-      <c r="J9">
-        <f>SUM(J3:J7)</f>
+      <c r="J9" s="4">
+        <f t="shared" si="4"/>
         <v>3868621098720.9995</v>
       </c>
-      <c r="K9">
-        <f>SUM(K3:K7)</f>
+      <c r="K9" s="5">
+        <f t="shared" si="4"/>
         <v>123795875159071.98</v>
       </c>
     </row>

</xml_diff>